<commit_message>
update 111 files and delete 40 files
</commit_message>
<xml_diff>
--- a/data/tehilim-data/100.xlsx
+++ b/data/tehilim-data/100.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>original</t>
   </si>
@@ -49,7 +49,13 @@
     <t>כָּל־הָאָרֶץ</t>
   </si>
   <si>
-    <t>вся земля</t>
+    <t xml:space="preserve">вся </t>
+  </si>
+  <si>
+    <t>הָאָרֶץ</t>
+  </si>
+  <si>
+    <t>земля</t>
   </si>
   <si>
     <t>ב</t>
@@ -585,19 +591,19 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2">
         <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10">
@@ -605,15 +611,15 @@
         <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -641,19 +647,19 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2">
         <v>3.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17">
@@ -682,15 +688,15 @@
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>36</v>
@@ -732,30 +738,30 @@
       <c r="A26" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="6">
+      <c r="A27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="6">
         <v>4.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30">
@@ -815,19 +821,19 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="6">
         <v>5.0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="39">
@@ -835,15 +841,15 @@
         <v>66</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41">
@@ -879,7 +885,12 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="7"/>
+      <c r="A45" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="7"/>
@@ -1024,6 +1035,9 @@
     </row>
     <row r="93">
       <c r="A93" s="7"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>